<commit_message>
company storage path update
</commit_message>
<xml_diff>
--- a/server/DATA/default_details/company_details.xlsx
+++ b/server/DATA/default_details/company_details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -98,36 +98,6 @@
     <t>PIPECO TANKS MALASIYA</t>
   </si>
   <si>
-    <t>apex</t>
-  </si>
-  <si>
-    <t>APEX TANKS TRADING L.L.C</t>
-  </si>
-  <si>
-    <t>APX</t>
-  </si>
-  <si>
-    <t>signs&amp;seals/apex_seal</t>
-  </si>
-  <si>
-    <t>apextanks.com</t>
-  </si>
-  <si>
-    <t>kings</t>
-  </si>
-  <si>
-    <t>kings TANKS TRADING L.L.C</t>
-  </si>
-  <si>
-    <t>KINGS</t>
-  </si>
-  <si>
-    <t>signs&amp;seals/kings_seal</t>
-  </si>
-  <si>
-    <t>kingstanks.com</t>
-  </si>
-  <si>
     <t>grp_template</t>
   </si>
   <si>
@@ -137,10 +107,16 @@
     <t>colex_template</t>
   </si>
   <si>
-    <t>apex_template</t>
-  </si>
-  <si>
-    <t>kings_template</t>
+    <t>company_storage_path</t>
+  </si>
+  <si>
+    <t>C:\Users\jovan\Downloads\grp_quotation_generator\server\Final_Doc/GRPT</t>
+  </si>
+  <si>
+    <t>C:\Users\jovan\Downloads\grp_quotation_generator\server\Final_Doc/GRPPT</t>
+  </si>
+  <si>
+    <t>C:\Users\jovan\Downloads\grp_quotation_generator\server\Final_Doc/CLX</t>
   </si>
 </sst>
 </file>
@@ -487,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,9 +474,10 @@
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
     <col min="6" max="6" width="23.77734375" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,13 +500,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -546,13 +526,16 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -569,13 +552,16 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -592,56 +578,13 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="H4" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>